<commit_message>
fix #2, especially 3 samples are due to method signature pattern (we can fix)
</commit_message>
<xml_diff>
--- a/datasets/CSV/sampled_unlinked_satd.xlsx
+++ b/datasets/CSV/sampled_unlinked_satd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="6440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="12900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sampled_unlinked_satd.ssv" sheetId="1" r:id="rId1"/>
@@ -569,42 +569,42 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>onStartElement(String,String,String,Attributes,AntXMLContext)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>src/main/org/apache/tools/ant/helper/ProjectHelper2.java</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>org.apache.tools.ant.helper.ProjectHelper2.ProjectHandler.onStartElement(String,String,String,Attributes,AntXMLContext)</t>
+  </si>
+  <si>
+    <t>proposal/sandbox/embed/RuntimeConfigurable2.java</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mapFileName(String)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t xml:space="preserve">This method was not deleted (494433) </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>onStartElement(String,String,String,Attributes,AntXMLContext)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>src/main/org/apache/tools/ant/helper/ProjectHelper2.java</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>org.apache.tools.ant.helper.ProjectHelper2.ProjectHandler.onStartElement(String,String,String,Attributes,AntXMLContext)</t>
-  </si>
-  <si>
-    <t>proposal/sandbox/embed/RuntimeConfigurable2.java</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>mapFileName(String)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1189,10 +1189,10 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1955,7 +1955,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -2033,7 +2033,7 @@
         <v>146</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" t="s">
         <v>146</v>
@@ -2119,19 +2119,19 @@
         <v>145</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>145</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>80</v>
@@ -2205,13 +2205,13 @@
         <v>145</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>145</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>79</v>
@@ -2291,7 +2291,7 @@
         <v>145</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>145</v>
@@ -2300,7 +2300,7 @@
         <v>145</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>89</v>
@@ -2377,7 +2377,7 @@
         <v>145</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>145</v>
@@ -2463,7 +2463,7 @@
         <v>145</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>145</v>
@@ -2555,7 +2555,7 @@
         <v>146</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>110</v>
@@ -2641,7 +2641,7 @@
         <v>146</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>117</v>
@@ -2721,7 +2721,7 @@
         <v>146</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>122</v>
@@ -2807,7 +2807,7 @@
         <v>146</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>130</v>
@@ -2887,13 +2887,13 @@
         <v>146</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H21" t="s">
         <v>117</v>
       </c>
       <c r="I21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>133</v>

</xml_diff>